<commit_message>
change in yml file
</commit_message>
<xml_diff>
--- a/DownloadExcel/CaseDetails.xlsx
+++ b/DownloadExcel/CaseDetails.xlsx
@@ -198,10 +198,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <cols>
     <col min="1" max="1" width="11.700000000000001" customWidth="1"/>
-    <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="10.4" customWidth="1"/>
+    <col min="2" max="2" width="16.900000000000002" customWidth="1"/>
+    <col min="3" max="3" width="11.700000000000001" customWidth="1"/>
     <col min="4" max="4" width="7.800000000000001" customWidth="1"/>
-    <col min="5" max="5" width="24.7" customWidth="1"/>
+    <col min="5" max="5" width="13" customWidth="1"/>
     <col min="6" max="6" width="26" customWidth="1"/>
     <col min="7" max="7" width="11.700000000000001" customWidth="1"/>
   </cols>
@@ -246,17 +246,17 @@
     <row r="2">
       <c t="inlineStr" r="A2">
         <is>
-          <t>CASE11589</t>
+          <t>CASE11591</t>
         </is>
       </c>
       <c t="inlineStr" r="B2">
         <is>
-          <t>Processing</t>
+          <t>Authorization</t>
         </is>
       </c>
       <c t="inlineStr" r="C2">
         <is>
-          <t>Rejected</t>
+          <t>Completed</t>
         </is>
       </c>
       <c t="inlineStr" r="D2">
@@ -266,12 +266,12 @@
       </c>
       <c t="inlineStr" r="E2">
         <is>
-          <t>Debashree Panigrahi</t>
+          <t>TEST USER</t>
         </is>
       </c>
       <c t="inlineStr" r="F2">
         <is>
-          <t>05-Jun-2024 06:04 PM</t>
+          <t>05-Jun-2024 06:46 PM</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Change in test logs
</commit_message>
<xml_diff>
--- a/DownloadExcel/CaseDetails.xlsx
+++ b/DownloadExcel/CaseDetails.xlsx
@@ -246,7 +246,7 @@
     <row r="2">
       <c t="inlineStr" r="A2">
         <is>
-          <t>CASE11600</t>
+          <t>CASE11611</t>
         </is>
       </c>
       <c t="inlineStr" r="B2">
@@ -271,7 +271,7 @@
       </c>
       <c t="inlineStr" r="F2">
         <is>
-          <t>06-Jun-2024 07:57 PM</t>
+          <t>07-Jun-2024 11:23 PM</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
change in pom file
</commit_message>
<xml_diff>
--- a/DownloadExcel/CaseDetails.xlsx
+++ b/DownloadExcel/CaseDetails.xlsx
@@ -246,7 +246,7 @@
     <row r="2">
       <c t="inlineStr" r="A2">
         <is>
-          <t>CASE329</t>
+          <t>CASE383</t>
         </is>
       </c>
       <c t="inlineStr" r="B2">
@@ -271,7 +271,7 @@
       </c>
       <c t="inlineStr" r="F2">
         <is>
-          <t>24-Sep-2024 07:07 PM</t>
+          <t>29-Oct-2024 09:07 AM</t>
         </is>
       </c>
     </row>

</xml_diff>